<commit_message>
Sensitivity for price correct forEOLRIR
</commit_message>
<xml_diff>
--- a/Results/Sensitivity/EOL-RIR/Lifetime/EOL_RIR_full_Lifetime_Max.xlsx
+++ b/Results/Sensitivity/EOL-RIR/Lifetime/EOL_RIR_full_Lifetime_Max.xlsx
@@ -414,13 +414,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.0001625819899935208</v>
+        <v>4.05721109302746E-07</v>
       </c>
       <c r="D2">
-        <v>0.5885782825730005</v>
+        <v>0.1664791307295803</v>
       </c>
       <c r="E2">
-        <v>0.6492109438477345</v>
+        <v>0.4065106765944204</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -428,16 +428,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2.183980475909258E-10</v>
+        <v>4.691044125953376E-13</v>
       </c>
       <c r="C3">
-        <v>0.007919668242014082</v>
+        <v>0.001512131801220273</v>
       </c>
       <c r="D3">
-        <v>0.5501068836496137</v>
+        <v>0.1058606147983076</v>
       </c>
       <c r="E3">
-        <v>0.5498836806399565</v>
+        <v>0.3596305710095618</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -445,16 +445,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3.409259119931335E-12</v>
+        <v>7.321669688613381E-15</v>
       </c>
       <c r="C4">
-        <v>0.00715402768698076</v>
+        <v>0.0003740244660593755</v>
       </c>
       <c r="D4">
-        <v>0.3927863988361095</v>
+        <v>0.07931982937362549</v>
       </c>
       <c r="E4">
-        <v>0.460358406415663</v>
+        <v>0.3171595483280041</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -465,13 +465,13 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1.587093575472108E-07</v>
+        <v>3.409138439013245E-10</v>
       </c>
       <c r="D5">
-        <v>0.02009765232936478</v>
+        <v>0.001223194692503424</v>
       </c>
       <c r="E5">
-        <v>0.03658129441505157</v>
+        <v>0.02413018472889736</v>
       </c>
     </row>
   </sheetData>
@@ -509,13 +509,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.0001842239112421771</v>
+        <v>4.057211093027732E-07</v>
       </c>
       <c r="D2">
-        <v>0.6669262277582069</v>
+        <v>0.1664791307295915</v>
       </c>
       <c r="E2">
-        <v>0.7356299384797864</v>
+        <v>0.4065106765944476</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -523,16 +523,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2.474698614308933E-10</v>
+        <v>4.691044125953693E-13</v>
       </c>
       <c r="C3">
-        <v>0.008973886094901615</v>
+        <v>0.001512131801220375</v>
       </c>
       <c r="D3">
-        <v>0.6233337512427775</v>
+        <v>0.1058606147983148</v>
       </c>
       <c r="E3">
-        <v>0.6230808368120845</v>
+        <v>0.3596305710095858</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -540,16 +540,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3.863078865850037E-12</v>
+        <v>7.321669688613872E-15</v>
       </c>
       <c r="C4">
-        <v>0.008106328146696585</v>
+        <v>0.0003740244660594007</v>
       </c>
       <c r="D4">
-        <v>0.4450717246061602</v>
+        <v>0.07931982937363082</v>
       </c>
       <c r="E4">
-        <v>0.5216385050182306</v>
+        <v>0.3171595483280256</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -560,13 +560,13 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1.798357776236215E-07</v>
+        <v>3.409138439013518E-10</v>
       </c>
       <c r="D5">
-        <v>0.02277292902521752</v>
+        <v>0.001223194692503522</v>
       </c>
       <c r="E5">
-        <v>0.0414507728421276</v>
+        <v>0.02413018472889929</v>
       </c>
     </row>
   </sheetData>
@@ -601,16 +601,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>6.556994183442194E-06</v>
+        <v>6.026889418659203E-07</v>
       </c>
       <c r="C2">
-        <v>0.005083743701291375</v>
+        <v>0.0002786503724174327</v>
       </c>
       <c r="D2">
-        <v>1.07580004858252</v>
+        <v>0.2533655906882806</v>
       </c>
       <c r="E2">
-        <v>0.9697180417558001</v>
+        <v>0.6996950518224571</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -618,16 +618,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.458740202226576E-05</v>
+        <v>4.096143759209795E-06</v>
       </c>
       <c r="C3">
-        <v>0.01839468255529511</v>
+        <v>0.005525867807623958</v>
       </c>
       <c r="D3">
-        <v>0.7727021730903773</v>
+        <v>0.15171349876109</v>
       </c>
       <c r="E3">
-        <v>0.6805195557530022</v>
+        <v>0.4843334564770065</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -635,16 +635,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.0001322419804487943</v>
+        <v>1.21620817902831E-05</v>
       </c>
       <c r="C4">
-        <v>0.004894520845755111</v>
+        <v>0.0007198594464809803</v>
       </c>
       <c r="D4">
-        <v>0.5532047049309021</v>
+        <v>0.09476617436401481</v>
       </c>
       <c r="E4">
-        <v>0.6055420661490584</v>
+        <v>0.4657667777509991</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -652,16 +652,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4.153988879660067E-05</v>
+        <v>3.819645484553135E-06</v>
       </c>
       <c r="C5">
-        <v>0.01081418683615371</v>
+        <v>0.001678931105475365</v>
       </c>
       <c r="D5">
-        <v>1.024873148138431</v>
+        <v>0.1708471635452753</v>
       </c>
       <c r="E5">
-        <v>0.7122850722825392</v>
+        <v>0.4717081075110235</v>
       </c>
     </row>
   </sheetData>
@@ -696,16 +696,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.966528370999151E-05</v>
+        <v>5.031589966768445E-06</v>
       </c>
       <c r="C2">
-        <v>0.003462735458016471</v>
+        <v>0.0003795813608333849</v>
       </c>
       <c r="D2">
-        <v>1.385766416475183</v>
+        <v>0.2641707319413292</v>
       </c>
       <c r="E2">
-        <v>1.39053799804532</v>
+        <v>1.383839401004388</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -713,16 +713,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.30035999530297E-05</v>
+        <v>5.367099139082082E-06</v>
       </c>
       <c r="C3">
-        <v>0.01164057132748931</v>
+        <v>0.001593037759322987</v>
       </c>
       <c r="D3">
-        <v>0.6708009055267363</v>
+        <v>0.1524988814736611</v>
       </c>
       <c r="E3">
-        <v>0.648446477114007</v>
+        <v>0.6174302220107619</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -730,16 +730,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.0003397047964529607</v>
+        <v>3.443534520072915E-05</v>
       </c>
       <c r="C4">
-        <v>0.003246107553390979</v>
+        <v>0.000412080869035601</v>
       </c>
       <c r="D4">
-        <v>0.6270289992800223</v>
+        <v>0.1111119351128833</v>
       </c>
       <c r="E4">
-        <v>0.7025531601665833</v>
+        <v>0.6154403591514438</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -747,16 +747,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.0001823860200208515</v>
+        <v>1.848515343462404E-05</v>
       </c>
       <c r="C5">
-        <v>0.004124207012744106</v>
+        <v>0.0005196111533190503</v>
       </c>
       <c r="D5">
-        <v>1.240009647204811</v>
+        <v>0.2361937477439512</v>
       </c>
       <c r="E5">
-        <v>0.9771097180398071</v>
+        <v>0.9816170507989759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>